<commit_message>
new Excel Model changes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDriver/ReferenceData/Revenue_RefData.xlsx
+++ b/src/test/resources/TestDriver/ReferenceData/Revenue_RefData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Transactions" sheetId="1" state="visible" r:id="rId3"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="60">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -79,133 +79,139 @@
     <t xml:space="preserve">Journal</t>
   </si>
   <si>
+    <t xml:space="preserve">Unbilled_Charge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New_Billing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Credit_Note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserField</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AttributeName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reclassable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Versionable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dataType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nullable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserField1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORDER_DATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserField2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITEM_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserField3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRODUCT_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserField4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SALE_PRICE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserField5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUANTITY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserField6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXTENDED_SALEPRICE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserField7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITEM_STARTDATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserField8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITEM_ENDDATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserField9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CURRENCY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserField10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRODUCT_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transaction Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metric Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unbilled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deferred_Revenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AccountSubType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AccountType</t>
+  </si>
+  <si>
     <t xml:space="preserve">Unbilled Charge</t>
   </si>
   <si>
-    <t xml:space="preserve">Revenue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Billing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Credit Note</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserField</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AttributeName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reclassable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Versionable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dataType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nullable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserField1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ORDER_DATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserField2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ITEM_ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserField3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRODUCT_ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserField4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SALE_PRICE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserField5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QUANTITY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserField6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXTENDED_SALEPRICE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserField7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ITEM_STARTDATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserField8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ITEM_ENDDATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserField9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CURRENCY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserField10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRODUCT_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transaction Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metric Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unbilled</t>
+    <t xml:space="preserve">Balance Sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Income Statement</t>
   </si>
   <si>
     <t xml:space="preserve">Deferred Revenue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AccountSubType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AccountType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Balance Sheet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Income Statement</t>
   </si>
   <si>
     <t xml:space="preserve">Contra Revenue</t>
@@ -604,11 +610,11 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="45.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.42"/>
@@ -635,7 +641,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>1</v>
@@ -649,7 +655,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>1</v>
@@ -960,15 +966,14 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="67.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="24.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16383" min="4" style="3" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="16384" style="3" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="3" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -990,7 +995,7 @@
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="str">
         <f aca="false">Transactions!A4</f>
-        <v>New Billing</v>
+        <v>New_Billing</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>40</v>
@@ -999,7 +1004,7 @@
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="str">
         <f aca="false">Transactions!A5</f>
-        <v>Credit Note</v>
+        <v>Credit_Note</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>40</v>
@@ -1008,7 +1013,7 @@
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="str">
         <f aca="false">Transactions!A2</f>
-        <v>Unbilled Charge</v>
+        <v>Unbilled_Charge</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>41</v>
@@ -1026,7 +1031,7 @@
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="str">
         <f aca="false">A3</f>
-        <v>New Billing</v>
+        <v>New_Billing</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>42</v>
@@ -1035,7 +1040,7 @@
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="str">
         <f aca="false">A4</f>
-        <v>Credit Note</v>
+        <v>Credit_Note</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>42</v>
@@ -1044,7 +1049,7 @@
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="str">
         <f aca="false">A5</f>
-        <v>Unbilled Charge</v>
+        <v>Unbilled_Charge</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>42</v>
@@ -1090,10 +1095,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1101,23 +1106,23 @@
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1140,7 +1145,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1154,16 +1159,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1171,10 +1176,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
@@ -1185,13 +1190,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1199,13 +1204,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1213,13 +1218,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1227,13 +1232,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1241,13 +1246,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1255,13 +1260,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1269,13 +1274,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1297,7 +1302,7 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1307,15 +1312,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="39.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16372" min="4" style="3" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="16379" style="3" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="16379" style="3" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>43</v>
@@ -1323,13 +1328,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="B2" s="9" t="n">
         <v>1000</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1345,42 +1350,42 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B4" s="9" t="n">
         <v>3000</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B5" s="9" t="n">
         <v>4000</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="1048561" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1390,10 +1395,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{f4c566ce-a3ce-4b10-b55b-1e9d56ad1b26}" enabled="0" method="" siteId="{f4c566ce-a3ce-4b10-b55b-1e9d56ad1b26}" removed="1"/>
-</clbl:labelList>
 </file>
</xml_diff>